<commit_message>
Nasar - 11Nov changes
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/OneCSiOS_TD.xlsx
+++ b/src/test/resources/test-data/OneCSiOS_TD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4989CB-2777-9146-A6B6-F1954A043703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDFDB8A-272A-CC4A-B7BE-ABF9E6045D72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>TESTDATA_KEY</t>
   </si>
@@ -86,6 +86,30 @@
   </si>
   <si>
     <t>A short, complete sentence that gives overview of the error.</t>
+  </si>
+  <si>
+    <t>CS_CREATE_A_SECURE</t>
+  </si>
+  <si>
+    <t>Charles Stanley. Create a secure financial future</t>
+  </si>
+  <si>
+    <t>Don't have an account?,Create one on our website</t>
+  </si>
+  <si>
+    <t>DON’T_HAVE_AN_ACCOUNT_LNK</t>
+  </si>
+  <si>
+    <t>CS_SECURE_URL</t>
+  </si>
+  <si>
+    <t>TESAT_DATA</t>
+  </si>
+  <si>
+    <t>SDFSDFDSFSDFDS</t>
+  </si>
+  <si>
+    <t>‎charles-stanley.co.uk, secure</t>
   </si>
 </sst>
 </file>
@@ -418,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -522,8 +546,40 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A11">
+  <conditionalFormatting sqref="A11:A15">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nasar - 14Nov changes
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/OneCSiOS_TD.xlsx
+++ b/src/test/resources/test-data/OneCSiOS_TD.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDFDB8A-272A-CC4A-B7BE-ABF9E6045D72}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831E05DB-468A-F94B-963F-52614C607E4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>TESTDATA_KEY</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Correct_Password</t>
   </si>
   <si>
-    <t>Alice</t>
-  </si>
-  <si>
     <t>Password123$</t>
   </si>
   <si>
@@ -110,6 +107,15 @@
   </si>
   <si>
     <t>‎charles-stanley.co.uk, secure</t>
+  </si>
+  <si>
+    <t>LETTER_A</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>incorrect</t>
   </si>
 </sst>
 </file>
@@ -442,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -479,7 +485,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -487,7 +493,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -495,7 +501,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -503,20 +509,20 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2">
         <v>123123</v>
@@ -524,62 +530,70 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A11:A15">
+  <conditionalFormatting sqref="A11:A16">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>